<commit_message>
Print only when X
</commit_message>
<xml_diff>
--- a/System_List_Example.xlsx
+++ b/System_List_Example.xlsx
@@ -1043,7 +1043,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:T168"/>
+  <dimension ref="B1:T181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9070,6 +9070,136 @@
         </is>
       </c>
     </row>
+    <row r="169">
+      <c r="B169" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>49000</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="B179" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="B181" t="n">
+        <v>30029017</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>